<commit_message>
List of dummy variables created during data preprocessing and reference categories and the list after removing statistically not important features
</commit_message>
<xml_diff>
--- a/List of dummy variables created during data_preprocessing.xlsx
+++ b/List of dummy variables created during data_preprocessing.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dummy variables for PD Model" sheetId="1" r:id="rId1"/>
     <sheet name="Reference categories" sheetId="2" r:id="rId2"/>
+    <sheet name="Significatnt variables on p_val" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="139">
   <si>
     <r>
       <t>'grade:B'</t>
@@ -1945,6 +1946,33 @@
       </rPr>
       <t>grade:G',</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"># we will look at the p-value of each dummy variable of independent features and we will remove the independent variables whose all </t>
+  </si>
+  <si>
+    <t># dummy variables have p-value &gt; 0.05</t>
+  </si>
+  <si>
+    <t># We do that by specifying another list of dummy variables as reference categories, and a list of variables to remove.</t>
+  </si>
+  <si>
+    <t># Then, we are going to drop the two datasets from the original list of dummy variables.</t>
+  </si>
+  <si>
+    <t># Variables</t>
+  </si>
+  <si>
+    <t>]]</t>
+  </si>
+  <si>
+    <t>are not statistically significant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># We are going to remove some features, the coefficients for all or almost all of the dummy variables which </t>
+  </si>
+  <si>
+    <t>grade:A',</t>
   </si>
 </sst>
 </file>
@@ -1952,13 +1980,6 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1977,6 +1998,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFCCCCCC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2002,10 +2029,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2288,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2940,7 +2968,7 @@
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3063,4 +3091,565 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="M109" sqref="M109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>